<commit_message>
fix errors in sbml expessions
</commit_message>
<xml_diff>
--- a/docs/function translation.xlsx
+++ b/docs/function translation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Heta</t>
   </si>
@@ -23,9 +23,6 @@
     <t>DBSolve</t>
   </si>
   <si>
-    <t>abs(x,y)</t>
-  </si>
-  <si>
     <t>add(x,y)</t>
   </si>
   <si>
@@ -153,6 +150,42 @@
   </si>
   <si>
     <t>ifeq(x, y, 1, 2)</t>
+  </si>
+  <si>
+    <t>SBML</t>
+  </si>
+  <si>
+    <t>ceiling(x)</t>
+  </si>
+  <si>
+    <t>abs(x)</t>
+  </si>
+  <si>
+    <t>plus</t>
+  </si>
+  <si>
+    <t>minus</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>divide</t>
+  </si>
+  <si>
+    <t>power(x,y)</t>
+  </si>
+  <si>
+    <t>root(x)</t>
+  </si>
+  <si>
+    <t>log_base(x)</t>
+  </si>
+  <si>
+    <t>log_2(x)</t>
+  </si>
+  <si>
+    <t>log(x) - natural</t>
   </si>
 </sst>
 </file>
@@ -509,281 +542,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="B1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="2" t="s">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update version and docs
</commit_message>
<xml_diff>
--- a/docs/function translation.xlsx
+++ b/docs/function translation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Heta</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>log(x) - natural</t>
+  </si>
+  <si>
+    <t>power(x,2)</t>
+  </si>
+  <si>
+    <t>ifg0(x-y, 1, 2)</t>
+  </si>
+  <si>
+    <t>ifge0(x-y, 1, 2)</t>
+  </si>
+  <si>
+    <t>ife0(x-y, 1, 2)</t>
   </si>
 </sst>
 </file>
@@ -544,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +775,7 @@
         <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
@@ -880,11 +892,17 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
       <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
@@ -894,12 +912,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
fix error in mrgsolve reaction output
</commit_message>
<xml_diff>
--- a/docs/function translation.xlsx
+++ b/docs/function translation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Heta</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>ife0(x-y, 1, 2)</t>
+  </si>
+  <si>
+    <t>sin(x), cos(x), tan(x), cot(x), sec(x), csc(x)</t>
+  </si>
+  <si>
+    <t>asin(x), acos(x), atan(x), acot(x), acsc(x), asec(x)</t>
+  </si>
+  <si>
+    <t>sinh(x), cosh(x), tanh(x), coth(x), sech(x), csch(x)</t>
+  </si>
+  <si>
+    <t>asinh(x), acosh(x), atanh(x), acoth(x), asech(x), acsch(x)</t>
+  </si>
+  <si>
+    <t>arcsinh(x), arccosh(x), arctanh(x), arccoth(x), arcsech(x), arccsch(x)</t>
+  </si>
+  <si>
+    <t>arcsin(x), arccos(x), arctan(x), arccot(x), arccsc(x), arcsec(x)</t>
   </si>
 </sst>
 </file>
@@ -228,12 +246,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -248,11 +290,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -554,15 +600,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E34"/>
+  <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="16.7265625" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
@@ -589,7 +635,7 @@
       <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -600,7 +646,7 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -611,7 +657,7 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -625,7 +671,7 @@
       <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -636,7 +682,7 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -647,7 +693,7 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -658,7 +704,7 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -669,7 +715,7 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -680,7 +726,7 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -691,7 +737,7 @@
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -702,7 +748,7 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -713,7 +759,7 @@
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -724,7 +770,7 @@
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -738,7 +784,7 @@
       <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -749,7 +795,7 @@
       <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -760,7 +806,7 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -774,7 +820,7 @@
       <c r="D19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -785,7 +831,7 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -912,17 +958,52 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function transformation to Julia
</commit_message>
<xml_diff>
--- a/docs/function translation.xlsx
+++ b/docs/function translation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Heta</t>
   </si>
@@ -216,6 +216,42 @@
   </si>
   <si>
     <t>arcsin(x), arccos(x), arctan(x), arccot(x), arccsc(x), arcsec(x)</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +(x,y)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /(x,y)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -(x,y)</t>
+  </si>
+  <si>
+    <t>*(x,y)</t>
+  </si>
+  <si>
+    <t>^(x,3)</t>
+  </si>
+  <si>
+    <t>^(x,2)</t>
+  </si>
+  <si>
+    <t>^(x,y)</t>
+  </si>
+  <si>
+    <t>log(base,x)</t>
+  </si>
+  <si>
+    <t>x-y == 0 ? 1 : 2</t>
+  </si>
+  <si>
+    <t>x-y &gt;= 0 ? 1 : 2</t>
+  </si>
+  <si>
+    <t>x-y &gt; 0 ? 1 : 2</t>
   </si>
 </sst>
 </file>
@@ -600,21 +636,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E39"/>
+  <dimension ref="B1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,8 +664,11 @@
       <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -638,8 +678,11 @@
       <c r="E3" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -649,8 +692,11 @@
       <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -660,8 +706,11 @@
       <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -674,8 +723,11 @@
       <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -685,8 +737,11 @@
       <c r="E7" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -696,8 +751,11 @@
       <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -707,8 +765,11 @@
       <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -718,8 +779,11 @@
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>56</v>
       </c>
@@ -729,8 +793,11 @@
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -740,8 +807,11 @@
       <c r="E12" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -751,8 +821,11 @@
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -762,8 +835,11 @@
       <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -773,8 +849,11 @@
       <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -787,8 +866,11 @@
       <c r="E16" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -798,8 +880,11 @@
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -809,8 +894,11 @@
       <c r="E18" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -823,19 +911,25 @@
       <c r="E19" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -845,8 +939,11 @@
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>35</v>
       </c>
@@ -856,8 +953,11 @@
       <c r="E22" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -867,8 +967,11 @@
       <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -878,8 +981,11 @@
       <c r="E24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -889,8 +995,11 @@
       <c r="E25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>29</v>
       </c>
@@ -900,8 +1009,11 @@
       <c r="E26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -911,8 +1023,11 @@
       <c r="E27" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -922,8 +1037,11 @@
       <c r="E28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>30</v>
       </c>
@@ -936,45 +1054,57 @@
       <c r="E29" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>61</v>
       </c>
@@ -982,7 +1112,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>62</v>
       </c>
@@ -990,7 +1120,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -998,7 +1128,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>64</v>
       </c>

</xml_diff>